<commit_message>
no more futur work
</commit_message>
<xml_diff>
--- a/Data/ArthurHeimCareerDataEn.xlsx
+++ b/Data/ArthurHeimCareerDataEn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthurheim/Library/CloudStorage/Dropbox/Travail_encrypted_decrypted/PHD/career/Data_DrivenResume/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D4A803-8E3A-E743-B99F-B58465EBC7ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D5B235-577B-B54E-8B14-9E0F5D089951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8220" yWindow="500" windowWidth="27240" windowHeight="19200" activeTab="9" xr2:uid="{65AA7443-0872-B84D-B38F-A133D7C4ED29}"/>
+    <workbookView xWindow="8220" yWindow="500" windowWidth="27240" windowHeight="19200" activeTab="2" xr2:uid="{65AA7443-0872-B84D-B38F-A133D7C4ED29}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="293">
   <si>
     <t>Degree</t>
   </si>
@@ -640,13 +640,7 @@
     <t>Trainer</t>
   </si>
   <si>
-    <t>IGPDE</t>
-  </si>
-  <si>
     <t>Training civil servants to public policy evaluation</t>
-  </si>
-  <si>
-    <t>EN3S</t>
   </si>
   <si>
     <t>Evaluating Public Health Policies: "New" Evaluation Methods.</t>
@@ -976,6 +970,27 @@
   </si>
   <si>
     <t>AFSE \&amp; DG Trésor</t>
+  </si>
+  <si>
+    <t>Strasbourg</t>
+  </si>
+  <si>
+    <t>Training futur high-level civil servants to public policy evaluation and anti-poverty policies</t>
+  </si>
+  <si>
+    <t>Institut national des études teritoriales (INET)</t>
+  </si>
+  <si>
+    <t>École nationale supérieure de la sécurité sociale (EN3S)</t>
+  </si>
+  <si>
+    <t>Institut de la gestion publique et du développement économique (IGPDE)</t>
+  </si>
+  <si>
+    <t>Participating in the evaluation of the effects of the national strategy to prevent and combat poverty, chaired by Louis Schweitzer.</t>
+  </si>
+  <si>
+    <t>Propose public policy initiatives focusing on the development, fulfilment and acquisition of young children.</t>
   </si>
 </sst>
 </file>
@@ -1100,7 +1115,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1147,6 +1162,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1520,13 +1536,13 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D2" t="s">
         <v>60</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="34">
@@ -1597,7 +1613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89004A4C-135E-AE46-AB58-A9B77E14C3A4}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1629,16 +1645,16 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E2" t="s">
         <v>117</v>
@@ -1650,16 +1666,16 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="28" t="s">
         <v>199</v>
-      </c>
-      <c r="D3" s="28" t="s">
-        <v>201</v>
       </c>
       <c r="E3" t="s">
         <v>116</v>
@@ -1679,7 +1695,7 @@
         <v>107</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E4" t="s">
         <v>115</v>
@@ -1710,7 +1726,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -1730,7 +1746,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B7" t="s">
         <v>114</v>
@@ -1750,7 +1766,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B8" t="s">
         <v>112</v>
@@ -1762,7 +1778,7 @@
         <v>121</v>
       </c>
       <c r="E8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F8" t="s">
         <v>23</v>
@@ -1770,7 +1786,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B9" t="s">
         <v>110</v>
@@ -1782,7 +1798,7 @@
         <v>120</v>
       </c>
       <c r="E9" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F9" t="s">
         <v>23</v>
@@ -1790,10 +1806,10 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B10" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C10" t="s">
         <v>107</v>
@@ -1810,7 +1826,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B11" t="s">
         <v>108</v>
@@ -1830,7 +1846,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B12" t="s">
         <v>105</v>
@@ -1907,7 +1923,7 @@
       </c>
       <c r="F2" s="18"/>
       <c r="G2" s="18" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1927,7 +1943,7 @@
         <v>84</v>
       </c>
       <c r="G3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2160,10 +2176,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8740F03-494A-C94E-AF3E-269AA0D15B6B}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2196,42 +2212,48 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>186</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>187</v>
-      </c>
-      <c r="C2" t="s">
-        <v>188</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>246</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="G2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="D2" s="5">
+        <v>2025</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="F2" t="s">
+        <v>287</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>190</v>
-      </c>
-      <c r="B3" t="s">
-        <v>189</v>
+        <v>186</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>187</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>188</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>247</v>
+        <v>245</v>
+      </c>
+      <c r="F3" t="s">
+        <v>292</v>
       </c>
       <c r="G3" t="s">
         <v>23</v>
@@ -2242,22 +2264,22 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B4" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>249</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>249</v>
+        <v>246</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>245</v>
       </c>
       <c r="F4" t="s">
-        <v>193</v>
+        <v>291</v>
       </c>
       <c r="G4" t="s">
         <v>23</v>
@@ -2271,19 +2293,19 @@
         <v>191</v>
       </c>
       <c r="B5" t="s">
-        <v>194</v>
+        <v>290</v>
       </c>
       <c r="C5" t="s">
         <v>107</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>249</v>
+        <v>157</v>
       </c>
       <c r="F5" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G5" t="s">
         <v>23</v>
@@ -2293,28 +2315,54 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="20"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="20"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="10"/>
+      <c r="A6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" t="s">
+        <v>289</v>
+      </c>
+      <c r="C6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="F6" t="s">
+        <v>193</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="20"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="20"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="20"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="10"/>
+      <c r="A12" s="10"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="20"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="20"/>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="10"/>
+      <c r="A15" s="10"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="20"/>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="20"/>
+      <c r="A18" s="10"/>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2359,7 +2407,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B3" t="s">
         <v>163</v>
@@ -2392,13 +2440,13 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B6" t="s">
         <v>166</v>
       </c>
       <c r="C6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2785,7 +2833,7 @@
         <v>70</v>
       </c>
       <c r="D6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E6">
         <v>2024</v>
@@ -2920,7 +2968,7 @@
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E2" s="24">
         <v>2024</v>
@@ -2952,7 +3000,7 @@
         <v>2024</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G3" s="24" t="s">
         <v>23</v>
@@ -3002,7 +3050,7 @@
         <v>2024</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G5" s="24" t="s">
         <v>23</v>
@@ -3014,13 +3062,13 @@
     <row r="6" spans="1:8" ht="221">
       <c r="A6" s="24"/>
       <c r="B6" s="24" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C6" s="24" t="s">
         <v>70</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E6" s="24">
         <v>2024</v>
@@ -3090,7 +3138,7 @@
         <v>128</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E9" s="24">
         <v>2024</v>
@@ -3123,7 +3171,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="17">
       <c r="A1" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>64</v>
@@ -3152,23 +3200,23 @@
     </row>
     <row r="2" spans="1:9" ht="136">
       <c r="A2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="24" t="s">
         <v>53</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F2" s="24">
         <v>2024</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H2" s="24" t="s">
         <v>23</v>
@@ -3179,11 +3227,11 @@
     </row>
     <row r="3" spans="1:9" ht="289">
       <c r="A3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B3" s="24"/>
       <c r="C3" s="24" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D3" s="24" t="s">
         <v>46</v>
@@ -3195,36 +3243,36 @@
         <v>2024</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H3" s="24" t="s">
         <v>23</v>
       </c>
       <c r="I3" s="24" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="119">
       <c r="A4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B4" s="24" t="s">
         <v>63</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F4" s="24">
         <v>2024</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H4" s="24" t="s">
         <v>23</v>
@@ -3235,11 +3283,11 @@
     </row>
     <row r="5" spans="1:9" ht="306">
       <c r="A5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B5" s="24"/>
       <c r="C5" s="24" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>52</v>
@@ -3251,7 +3299,7 @@
         <v>2024</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="H5" s="24" t="s">
         <v>23</v>
@@ -3262,23 +3310,23 @@
     </row>
     <row r="6" spans="1:9" ht="170">
       <c r="A6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B6" s="24"/>
       <c r="C6" s="24" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D6" s="24" t="s">
         <v>70</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F6" s="24">
         <v>2024</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H6" s="24" t="s">
         <v>23</v>
@@ -3335,7 +3383,7 @@
     </row>
     <row r="9" spans="1:9" ht="85">
       <c r="A9" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B9" s="24"/>
       <c r="C9" s="26" t="s">
@@ -3345,13 +3393,13 @@
         <v>128</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F9" s="24">
         <v>2024</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H9" s="24" t="s">
         <v>23</v>
@@ -3382,7 +3430,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>16</v>
@@ -3403,174 +3451,174 @@
         <v>21</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>249</v>
+      </c>
+      <c r="F2" t="s">
+        <v>209</v>
+      </c>
+      <c r="G2" t="s">
         <v>216</v>
       </c>
-      <c r="B2" t="s">
-        <v>223</v>
-      </c>
-      <c r="C2" t="s">
-        <v>206</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>250</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>251</v>
-      </c>
-      <c r="F2" t="s">
-        <v>211</v>
-      </c>
-      <c r="G2" t="s">
-        <v>218</v>
-      </c>
       <c r="H2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B5" t="s">
         <v>221</v>
       </c>
-      <c r="B5" t="s">
-        <v>223</v>
-      </c>
       <c r="C5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F6" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E7" s="27" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G7" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B8" t="s">
         <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D8">
         <v>2013</v>
@@ -3579,24 +3627,24 @@
         <v>2014</v>
       </c>
       <c r="F8" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G8" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H8" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B9" t="s">
         <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D9">
         <v>2014</v>
@@ -3605,13 +3653,13 @@
         <v>2016</v>
       </c>
       <c r="F9" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G9" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H9" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>